<commit_message>
lexin's wrk, final touches
</commit_message>
<xml_diff>
--- a/main/backend/Municipal_Data_Inventory.xlsx
+++ b/main/backend/Municipal_Data_Inventory.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K2"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -451,71 +451,69 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>dataset_name</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>description</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>department</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>format</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>update_frequency</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>public</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>metadata_status</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>notes</t>
+          <t>uploaded</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
+          <t>FY25 original, 1st amendment and FY26 original Budgets.xlsx</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>xlsx</t>
+        </is>
+      </c>
+      <c r="C2" t="n">
+        <v>37.63</v>
+      </c>
+      <c r="D2" t="inlineStr">
+        <is>
+          <t>2025-11-06 14:44:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Municipal_Data_Inventory.xlsx</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>xlsx</t>
+        </is>
+      </c>
+      <c r="C3" t="n">
+        <v>5.02</v>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>2025-11-06 15:12:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" t="inlineStr">
+        <is>
           <t>ALL FY25 Budgets.xlsx</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>application/vnd.openxmlformats-officedocument.spreadsheetml.sheet</t>
-        </is>
-      </c>
-      <c r="C2" t="n">
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>xlsx</t>
+        </is>
+      </c>
+      <c r="C4" t="n">
         <v>26.12</v>
       </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>asd</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr"/>
-      <c r="F2" t="inlineStr"/>
-      <c r="G2" t="inlineStr"/>
-      <c r="H2" t="inlineStr"/>
-      <c r="I2" t="inlineStr"/>
-      <c r="J2" t="inlineStr"/>
-      <c r="K2" t="inlineStr"/>
+      <c r="D4" t="inlineStr">
+        <is>
+          <t>2025-11-06 14:48:39</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>